<commit_message>
Chore(Routes): Updating PUT - POST Routes Configuration
</commit_message>
<xml_diff>
--- a/Docs/Routes Mapping.xlsx
+++ b/Docs/Routes Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv00wyv\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv00wyv\Desktop\P_Bulle_Dev_FlashCards\latest\P_Bulle_Dev-Flashcards\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44003DD-2DEC-43E6-806C-12D0B80FDC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE800B2-5492-455D-9ABE-9242402CE623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{78FF3FEE-8393-407A-AC41-6BC005ADEBC8}"/>
   </bookViews>
@@ -194,9 +194,6 @@
     <t>Lister toutes les flashcards d’un deck</t>
   </si>
   <si>
-    <t>/cards/:id</t>
-  </si>
-  <si>
     <t>Voir une flashcard</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>Score, stats, option rejouer</t>
+  </si>
+  <si>
+    <t>/decks/:deckId/cards/:cardId</t>
   </si>
 </sst>
 </file>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADC9317-4E1B-4E09-9554-13BC2DDA84E4}">
   <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -957,7 +957,7 @@
     </row>
     <row r="26" spans="2:5" ht="31.5">
       <c r="B26" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="2:5">
@@ -993,10 +993,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>39</v>
@@ -1010,7 +1010,7 @@
         <v>50</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>41</v>
@@ -1021,10 +1021,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>39</v>
@@ -1035,10 +1035,10 @@
         <v>2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>39</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="35" spans="2:5" ht="31.5">
       <c r="B35" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="2:5">
@@ -1068,13 +1068,13 @@
         <v>0</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -1082,13 +1082,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="39" spans="2:5">
@@ -1096,13 +1096,13 @@
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="40" spans="2:5">
@@ -1110,13 +1110,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>